<commit_message>
completed webpage and web api authorization
</commit_message>
<xml_diff>
--- a/DDL.xlsx
+++ b/DDL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\C# Training\Final_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF3099EA-7A4E-4FA8-82DC-6241E52C1B02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23EA9B45-6189-426B-9D23-C2F6C5B82F2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="360" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tables for the project" sheetId="12" r:id="rId1"/>
@@ -718,7 +718,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E15045E-5C25-48D1-9471-98A2E828D8C0}">
   <dimension ref="X1:Y29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+    <sheetView topLeftCell="S6" workbookViewId="0">
       <selection activeCell="X14" sqref="X14"/>
     </sheetView>
   </sheetViews>
@@ -1814,7 +1814,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="Q1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
@@ -2458,9 +2458,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="14.90625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">

</xml_diff>